<commit_message>
I modified homework's exercise
</commit_message>
<xml_diff>
--- a/appunti/Glossario.xlsx
+++ b/appunti/Glossario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi\Desktop\4AROB\sistemi-Reti\appunti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90AD396-4D97-4057-84CF-73CA8D5B0124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A13D99-2E76-4E64-8ED7-17648388B423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3B0C8353-AE24-4107-B227-A59564D08BC4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>TERMINI</t>
   </si>
@@ -235,6 +235,72 @@
   </si>
   <si>
     <t>Service Set Identifier: non è nient'altro che un nome della rete wireless di un utente. Noto anche come ID di rete, è una rete wireless visualizzabile da chiunque.</t>
+  </si>
+  <si>
+    <t>livello</t>
+  </si>
+  <si>
+    <t>layer</t>
+  </si>
+  <si>
+    <t>protocol</t>
+  </si>
+  <si>
+    <t>protocollo</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>legge di metcalfe</t>
+  </si>
+  <si>
+    <t>payload</t>
+  </si>
+  <si>
+    <t>livelli iso/osi</t>
+  </si>
+  <si>
+    <t>livelli tcp/ip</t>
+  </si>
+  <si>
+    <t>flow control</t>
+  </si>
+  <si>
+    <t>data order</t>
+  </si>
+  <si>
+    <t>ieee vari</t>
+  </si>
+  <si>
+    <t>spoofing</t>
+  </si>
+  <si>
+    <t>multicast</t>
+  </si>
+  <si>
+    <t>ethernet</t>
+  </si>
+  <si>
+    <t>type field</t>
+  </si>
+  <si>
+    <t>vlan tag</t>
+  </si>
+  <si>
+    <t>sfd</t>
+  </si>
+  <si>
+    <t>bande</t>
+  </si>
+  <si>
+    <t>BSS</t>
+  </si>
+  <si>
+    <t>ESS</t>
+  </si>
+  <si>
+    <t>datagrammi</t>
   </si>
 </sst>
 </file>
@@ -284,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -293,9 +359,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -612,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D28CCC50-9CBF-4693-B669-59F43FCCD1C6}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,7 +736,7 @@
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -824,7 +887,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -857,34 +920,140 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>